<commit_message>
maj gantt et diagramme exi
</commit_message>
<xml_diff>
--- a/GANTT Projet WEB.xlsx
+++ b/GANTT Projet WEB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Twitter Damien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{E0C445FF-DACF-490C-9633-5E2FD43BE706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,66 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <t>PLAN START</t>
@@ -153,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,7 +383,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,9 +408,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -505,28 +444,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
@@ -535,27 +480,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="% complete" xfId="16"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
+    <cellStyle name="Activity" xfId="2"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
+    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Percent Complete" xfId="6"/>
+    <cellStyle name="Period Headers" xfId="3"/>
+    <cellStyle name="Period Highlight Control" xfId="7"/>
+    <cellStyle name="Period Value" xfId="13"/>
+    <cellStyle name="Plan legend" xfId="14"/>
+    <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Texte explicatif" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Titre" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -945,118 +884,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AK30"/>
+  <dimension ref="B1:AK31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="26.25" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="4" customWidth="1"/>
     <col min="8" max="8" width="2.75" style="1" customWidth="1"/>
     <col min="9" max="27" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
-      <c r="B1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="2:37" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+    <row r="1" spans="2:37" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="2:37" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="30"/>
-    </row>
-    <row r="3" spans="2:37" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="31"/>
+    </row>
+    <row r="3" spans="2:37" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-    </row>
-    <row r="4" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+    </row>
+    <row r="4" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1148,9 +1087,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:37" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:37" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -1164,13 +1103,13 @@
       <c r="F5" s="7">
         <v>5</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1184,13 +1123,13 @@
       <c r="F6" s="7">
         <v>5</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:37" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:37" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -1204,13 +1143,13 @@
       <c r="F7" s="7">
         <v>10</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7">
         <v>16</v>
@@ -1224,13 +1163,13 @@
       <c r="F8" s="7">
         <v>2</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:37" ht="32.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:37" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1244,13 +1183,13 @@
       <c r="F9" s="7">
         <v>12</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:37" ht="45.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:37" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7">
         <v>18</v>
@@ -1264,13 +1203,13 @@
       <c r="F10" s="7">
         <v>13</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:37" ht="50" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:37" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1284,413 +1223,588 @@
       <c r="F11" s="7">
         <v>13</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0</v>
-      </c>
-      <c r="G24" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7">
-        <v>0</v>
-      </c>
-      <c r="G25" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="7">
-        <v>0</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="7">
-        <v>0</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="32">
-        <v>0</v>
-      </c>
+    <row r="12" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+    </row>
+    <row r="13" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+    </row>
+    <row r="14" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+    </row>
+    <row r="16" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+    </row>
+    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+    </row>
+    <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+    </row>
+    <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+    </row>
+    <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+    </row>
+    <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+    </row>
+    <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+    </row>
+    <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+    </row>
+    <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+    </row>
+    <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+    </row>
+    <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+    </row>
+    <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+    </row>
+    <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+    </row>
+    <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+    </row>
+    <row r="30" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+    </row>
+    <row r="31" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="S2:W2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="S2:W2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B31:AK31">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H4:AK4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:AK30">
+  <conditionalFormatting sqref="H5:AK11">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1717,22 +1831,22 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="J2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="O2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="R2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="J2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="O2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="R2"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
maj msg error insc
</commit_message>
<xml_diff>
--- a/GANTT Projet WEB.xlsx
+++ b/GANTT Projet WEB.xlsx
@@ -36,24 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>PLAN START</t>
-  </si>
-  <si>
-    <t>PLAN DURATION</t>
-  </si>
-  <si>
-    <t>ACTUAL START</t>
-  </si>
-  <si>
-    <t>ACTUAL DURATION</t>
-  </si>
-  <si>
-    <t>PERCENT COMPLETE</t>
   </si>
   <si>
     <t>Faire la page d'inscription/connexion</t>
@@ -999,7 +984,7 @@
   <dimension ref="B1:AK31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AM10" sqref="AM10"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1017,7 +1002,7 @@
   <sheetData>
     <row r="1" spans="2:37" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -1032,24 +1017,24 @@
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H2" s="13"/>
       <c r="J2" s="15"/>
       <c r="K2" s="23" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
       <c r="N2" s="25"/>
       <c r="O2" s="16"/>
       <c r="P2" s="18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="19"/>
       <c r="R2" s="14"/>
       <c r="S2" s="23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="T2" s="26"/>
       <c r="U2" s="26"/>
@@ -1060,21 +1045,11 @@
       <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="17"/>
       <c r="I3" s="8"/>
       <c r="J3" s="9"/>
@@ -1196,7 +1171,7 @@
     </row>
     <row r="5" spans="2:37" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -1216,7 +1191,7 @@
     </row>
     <row r="6" spans="2:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1236,7 +1211,7 @@
     </row>
     <row r="7" spans="2:37" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -1256,7 +1231,7 @@
     </row>
     <row r="8" spans="2:37" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7">
         <v>16</v>
@@ -1276,7 +1251,7 @@
     </row>
     <row r="9" spans="2:37" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1296,7 +1271,7 @@
     </row>
     <row r="10" spans="2:37" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7">
         <v>18</v>
@@ -1316,7 +1291,7 @@
     </row>
     <row r="11" spans="2:37" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1336,7 +1311,7 @@
     </row>
     <row r="12" spans="2:37" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>25</v>

</xml_diff>